<commit_message>
atualização da base 17h25
</commit_message>
<xml_diff>
--- a/data/csa_pindorama.xlsx
+++ b/data/csa_pindorama.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RNFAVAR.EMBAD.000\Documents\NEO DIPAS\Ciencia de Dados na Embraer\repos\web_app_CSA_pindorama\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017B3D31-7A2F-492B-95E5-D8E6773C2FC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91400C74-FB33-4453-A481-600940934482}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15660" xr2:uid="{45442450-1535-414E-8E8C-F2E9142920AB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>produto</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>rúcula</t>
+  </si>
+  <si>
+    <t>mexerica ponkan</t>
+  </si>
+  <si>
+    <t>hortelã</t>
   </si>
 </sst>
 </file>
@@ -424,15 +430,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C165D6F-8FA7-44DB-A078-36B533BEFB91}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -535,6 +541,25 @@
         <v>3</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
atualização da base 17h33
</commit_message>
<xml_diff>
--- a/data/csa_pindorama.xlsx
+++ b/data/csa_pindorama.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RNFAVAR.EMBAD.000\Documents\NEO DIPAS\Ciencia de Dados na Embraer\repos\web_app_CSA_pindorama\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91400C74-FB33-4453-A481-600940934482}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333F28D3-A5FB-4194-BB89-D658136C7EFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15660" xr2:uid="{45442450-1535-414E-8E8C-F2E9142920AB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
   <si>
     <t>produto</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>hortelã</t>
+  </si>
+  <si>
+    <t>pepino</t>
   </si>
 </sst>
 </file>
@@ -430,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C165D6F-8FA7-44DB-A078-36B533BEFB91}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,6 +563,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
atualização do app e da base de dados
</commit_message>
<xml_diff>
--- a/data/csa_pindorama.xlsx
+++ b/data/csa_pindorama.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RNFAVAR.EMBAD.000\Documents\NEO DIPAS\Ciencia de Dados na Embraer\repos\web_app_CSA_pindorama\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B877E4B-2057-4D86-B602-C1CB3566815F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F623B19C-B240-4E46-8D72-A682A259D3D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15660" xr2:uid="{45442450-1535-414E-8E8C-F2E9142920AB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="produtos" sheetId="1" r:id="rId1"/>
+    <sheet name="busca_cesta" sheetId="2" r:id="rId2"/>
+    <sheet name="mutiroes" sheetId="4" r:id="rId3"/>
+    <sheet name="info_nutricional" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="142">
   <si>
     <t>produto</t>
   </si>
@@ -45,9 +48,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>banana</t>
-  </si>
-  <si>
     <t>mandioca</t>
   </si>
   <si>
@@ -57,15 +57,6 @@
     <t>alface crespa</t>
   </si>
   <si>
-    <t>escarola</t>
-  </si>
-  <si>
-    <t>espinafre</t>
-  </si>
-  <si>
-    <t>acelga</t>
-  </si>
-  <si>
     <t>beterraba</t>
   </si>
   <si>
@@ -81,18 +72,410 @@
     <t>hortelã</t>
   </si>
   <si>
-    <t>pepino</t>
-  </si>
-  <si>
-    <t>uva</t>
+    <t>pimenta biquinho</t>
+  </si>
+  <si>
+    <t>amora</t>
+  </si>
+  <si>
+    <t>acerola</t>
+  </si>
+  <si>
+    <t>banana prata</t>
+  </si>
+  <si>
+    <t>banana nanina</t>
+  </si>
+  <si>
+    <t>banana marmelo/figo/pão</t>
+  </si>
+  <si>
+    <t>ervilha torta</t>
+  </si>
+  <si>
+    <t>tomate</t>
+  </si>
+  <si>
+    <t>coentro</t>
+  </si>
+  <si>
+    <t>salsinha</t>
+  </si>
+  <si>
+    <t>cebolinha</t>
+  </si>
+  <si>
+    <t>brócolis</t>
+  </si>
+  <si>
+    <t>couve-flor</t>
+  </si>
+  <si>
+    <t>couve manteiga</t>
+  </si>
+  <si>
+    <t>manga</t>
+  </si>
+  <si>
+    <t>morango</t>
+  </si>
+  <si>
+    <t>alho poró</t>
+  </si>
+  <si>
+    <t>hortelã pimenta</t>
+  </si>
+  <si>
+    <t>figo</t>
+  </si>
+  <si>
+    <t>feijão guandu</t>
+  </si>
+  <si>
+    <t>peixinho</t>
+  </si>
+  <si>
+    <t>azedinha</t>
+  </si>
+  <si>
+    <t>ora-pro-nóbis</t>
+  </si>
+  <si>
+    <t>laranja</t>
+  </si>
+  <si>
+    <t>alecrim</t>
+  </si>
+  <si>
+    <t>manjericão</t>
+  </si>
+  <si>
+    <t>chaya/árvore de espinafre</t>
+  </si>
+  <si>
+    <t>pimentão</t>
+  </si>
+  <si>
+    <t>salsão</t>
+  </si>
+  <si>
+    <t>limão cravo</t>
+  </si>
+  <si>
+    <t>alfavaca</t>
+  </si>
+  <si>
+    <t>goiaba vermelha</t>
+  </si>
+  <si>
+    <t>goiaba branca</t>
+  </si>
+  <si>
+    <t>gengibre</t>
+  </si>
+  <si>
+    <t>colorau/pó de urucum</t>
+  </si>
+  <si>
+    <t>Ana Beatriz</t>
+  </si>
+  <si>
+    <t>Débora/Humberto</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Alimento</t>
+  </si>
+  <si>
+    <t>Gramas</t>
+  </si>
+  <si>
+    <t>Calorias</t>
+  </si>
+  <si>
+    <t>Proteína</t>
+  </si>
+  <si>
+    <t>Fibra</t>
+  </si>
+  <si>
+    <t>Carboidrato</t>
+  </si>
+  <si>
+    <t>Alcachofra</t>
+  </si>
+  <si>
+    <t>100.0</t>
+  </si>
+  <si>
+    <t>44.0</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>10.0</t>
+  </si>
+  <si>
+    <t>Aspargo</t>
+  </si>
+  <si>
+    <t>96.0</t>
+  </si>
+  <si>
+    <t>18.0</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>Feijão</t>
+  </si>
+  <si>
+    <t>125.0</t>
+  </si>
+  <si>
+    <t>25.0</t>
+  </si>
+  <si>
+    <t>0.8</t>
+  </si>
+  <si>
+    <t>6.0</t>
+  </si>
+  <si>
+    <t>Lima</t>
+  </si>
+  <si>
+    <t>160.0</t>
+  </si>
+  <si>
+    <t>140.0</t>
+  </si>
+  <si>
+    <t>8.0</t>
+  </si>
+  <si>
+    <t>24.0</t>
+  </si>
+  <si>
+    <t>Broto de feijão</t>
+  </si>
+  <si>
+    <t>50.0</t>
+  </si>
+  <si>
+    <t>17.0</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>Folhas de beterraba</t>
+  </si>
+  <si>
+    <t>27.0</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>Beterraba</t>
+  </si>
+  <si>
+    <t>43.0</t>
+  </si>
+  <si>
+    <t>12.0</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>Brócolis</t>
+  </si>
+  <si>
+    <t>150.0</t>
+  </si>
+  <si>
+    <t>45.0</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>1.9</t>
+  </si>
+  <si>
+    <t>Couve de bruxelas</t>
+  </si>
+  <si>
+    <t>130.0</t>
+  </si>
+  <si>
+    <t>60.0</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t>Cenouras</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>Couve-flor</t>
+  </si>
+  <si>
+    <t>120.0</t>
+  </si>
+  <si>
+    <t>30.0</t>
+  </si>
+  <si>
+    <t>Salsão</t>
+  </si>
+  <si>
+    <t>20.0</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>Milho</t>
+  </si>
+  <si>
+    <t>92.0</t>
+  </si>
+  <si>
+    <t>21.0</t>
+  </si>
+  <si>
+    <t>Pepino</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>Melancia</t>
+  </si>
+  <si>
+    <t>925.0</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>29.0</t>
+  </si>
+  <si>
+    <t>Batata doce</t>
+  </si>
+  <si>
+    <t>110.0</t>
+  </si>
+  <si>
+    <t>155.0</t>
+  </si>
+  <si>
+    <t>36.0</t>
+  </si>
+  <si>
+    <t>Ervilhas</t>
+  </si>
+  <si>
+    <t>66.0</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>13.0</t>
+  </si>
+  <si>
+    <t>Alface</t>
+  </si>
+  <si>
+    <t>14.0</t>
+  </si>
+  <si>
+    <t>Couve</t>
+  </si>
+  <si>
+    <t>Berinjela</t>
+  </si>
+  <si>
+    <t>180.0</t>
+  </si>
+  <si>
+    <t>9.0</t>
+  </si>
+  <si>
+    <t>Tomate</t>
+  </si>
+  <si>
+    <t>240.0</t>
+  </si>
+  <si>
+    <t>29/mai</t>
+  </si>
+  <si>
+    <t>06/jun</t>
+  </si>
+  <si>
+    <t>batata tupinambo/ alcachofra-girassol/ girassol-batateiro</t>
+  </si>
+  <si>
+    <t>bertalha/ espinafre indiano</t>
+  </si>
+  <si>
+    <t>chingensai/ bok choi/ acelga chinesa</t>
+  </si>
+  <si>
+    <t>cúrcuma/ açafrão-da-terra/ açafrão-da-índia</t>
+  </si>
+  <si>
+    <t>hibisco/ vinagreira/ quiabo-azedo</t>
+  </si>
+  <si>
+    <t>tomate cereja/ tomatinho</t>
+  </si>
+  <si>
+    <t>30/mai</t>
+  </si>
+  <si>
+    <t>preparo de novos canteiros</t>
+  </si>
+  <si>
+    <t>Marina/Renato, ???</t>
+  </si>
+  <si>
+    <t>pimenta-cambuci/ pimentão-chapéu-de-bispo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -120,8 +503,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,31 +821,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C165D6F-8FA7-44DB-A078-36B533BEFB91}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -473,24 +858,18 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -501,12 +880,15 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -514,12 +896,15 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -527,40 +912,31 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>132</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
@@ -568,7 +944,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>133</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
@@ -576,13 +952,858 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>134</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>136</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>141</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>137</v>
+      </c>
+      <c r="B51" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C51">
+    <sortCondition ref="A51"/>
+  </sortState>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A844EE-D887-4A6B-B86C-B7C752CAF55A}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72601697-55EE-475A-BC70-2B6BB9EC57DD}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF289E3-7000-4F49-BDDB-76D25F29B57D}">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" t="s">
+        <v>120</v>
+      </c>
+      <c r="F14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F22">
+    <sortCondition ref="A2"/>
+  </sortState>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
atualização da base e do app
</commit_message>
<xml_diff>
--- a/data/csa_pindorama.xlsx
+++ b/data/csa_pindorama.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RNFAVAR.EMBAD.000\Documents\NEO DIPAS\Ciencia de Dados na Embraer\repos\web_app_CSA_pindorama\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE05219-5366-4FB1-857A-96A3AD8A1D4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B0B3E2-8478-40C3-9172-9F9E39C08D1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15660" xr2:uid="{45442450-1535-414E-8E8C-F2E9142920AB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="146">
   <si>
     <t>produto</t>
   </si>
@@ -466,6 +466,12 @@
   </si>
   <si>
     <t>banana nanica</t>
+  </si>
+  <si>
+    <t>espinfre</t>
+  </si>
+  <si>
+    <t>caju</t>
   </si>
 </sst>
 </file>
@@ -827,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C165D6F-8FA7-44DB-A078-36B533BEFB91}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,26 +988,26 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>133</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
@@ -1009,7 +1015,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
@@ -1017,7 +1023,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
@@ -1025,7 +1031,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
@@ -1033,7 +1039,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
@@ -1041,7 +1047,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>134</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
@@ -1049,7 +1055,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
@@ -1057,7 +1063,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
         <v>3</v>
@@ -1065,7 +1071,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>144</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
@@ -1073,18 +1079,15 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
@@ -1092,15 +1095,18 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>43</v>
       </c>
       <c r="B32" t="s">
         <v>3</v>
@@ -1108,7 +1114,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="B33" t="s">
         <v>3</v>
@@ -1116,7 +1122,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>135</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
@@ -1124,7 +1130,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>141</v>
+        <v>11</v>
       </c>
       <c r="B35" t="s">
         <v>3</v>
@@ -1132,7 +1138,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B36" t="s">
         <v>3</v>
@@ -1140,18 +1146,15 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>141</v>
       </c>
       <c r="B37" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="B38" t="s">
         <v>3</v>
@@ -1159,15 +1162,18 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="B40" t="s">
         <v>3</v>
@@ -1175,18 +1181,15 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B41" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B42" t="s">
         <v>3</v>
@@ -1194,15 +1197,18 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="B43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B44" t="s">
         <v>3</v>
@@ -1210,7 +1216,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="B45" t="s">
         <v>3</v>
@@ -1218,18 +1224,15 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>140</v>
+        <v>31</v>
       </c>
       <c r="B46" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B47" t="s">
         <v>3</v>
@@ -1237,15 +1240,18 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>8</v>
+        <v>140</v>
       </c>
       <c r="B48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B49" t="s">
         <v>3</v>
@@ -1253,7 +1259,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B50" t="s">
         <v>3</v>
@@ -1261,18 +1267,15 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B51" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="B52" t="s">
         <v>3</v>
@@ -1280,15 +1283,34 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>18</v>
+      </c>
+      <c r="B54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>136</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B55" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C53">
-    <sortCondition ref="A53"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C55">
+    <sortCondition ref="A35"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
atualização da base e do aplicativo
</commit_message>
<xml_diff>
--- a/data/csa_pindorama.xlsx
+++ b/data/csa_pindorama.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RNFAVAR.EMBAD.000\Documents\NEO DIPAS\Ciencia de Dados na Embraer\repos\web_app_CSA_pindorama\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD779EA-8558-445E-BB01-26783B449598}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24848C3D-F61E-4BC0-A829-0BF31FE27AC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15660" activeTab="2" xr2:uid="{45442450-1535-414E-8E8C-F2E9142920AB}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15660" xr2:uid="{45442450-1535-414E-8E8C-F2E9142920AB}"/>
   </bookViews>
   <sheets>
     <sheet name="produtos" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="265">
   <si>
     <t>produto</t>
   </si>
@@ -241,9 +241,6 @@
     <t>banana nanica</t>
   </si>
   <si>
-    <t>espinfre</t>
-  </si>
-  <si>
     <t>caju</t>
   </si>
   <si>
@@ -448,15 +445,6 @@
     <t>vitamina c (mg)</t>
   </si>
   <si>
-    <t>carboidrato (g)</t>
-  </si>
-  <si>
-    <t>fibra (g)</t>
-  </si>
-  <si>
-    <t>proteína (g)</t>
-  </si>
-  <si>
     <t>calorias (kcal)</t>
   </si>
   <si>
@@ -467,6 +455,401 @@
   </si>
   <si>
     <t>03/jun</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>carro 1</t>
+  </si>
+  <si>
+    <t>carro 2</t>
+  </si>
+  <si>
+    <t>participantes</t>
+  </si>
+  <si>
+    <t>bertalha</t>
+  </si>
+  <si>
+    <t>cabeludinha</t>
+  </si>
+  <si>
+    <t>chaya</t>
+  </si>
+  <si>
+    <t>chingensai</t>
+  </si>
+  <si>
+    <t>colorau</t>
+  </si>
+  <si>
+    <t>objetivo</t>
+  </si>
+  <si>
+    <t>35.3</t>
+  </si>
+  <si>
+    <t>5.42</t>
+  </si>
+  <si>
+    <t>3.02</t>
+  </si>
+  <si>
+    <t>cúrcuma</t>
+  </si>
+  <si>
+    <t>1.92</t>
+  </si>
+  <si>
+    <t>48.2</t>
+  </si>
+  <si>
+    <t>11.43</t>
+  </si>
+  <si>
+    <t>3.9</t>
+  </si>
+  <si>
+    <t>65.37</t>
+  </si>
+  <si>
+    <t>80.8</t>
+  </si>
+  <si>
+    <t>9.7</t>
+  </si>
+  <si>
+    <t>7.5</t>
+  </si>
+  <si>
+    <t>14.2</t>
+  </si>
+  <si>
+    <t>12.4</t>
+  </si>
+  <si>
+    <t>espinafre</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>3.63</t>
+  </si>
+  <si>
+    <t>28.1</t>
+  </si>
+  <si>
+    <t>21.7</t>
+  </si>
+  <si>
+    <t>62.78</t>
+  </si>
+  <si>
+    <t>23.88</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>7.2</t>
+  </si>
+  <si>
+    <t>0.75</t>
+  </si>
+  <si>
+    <t>2.9</t>
+  </si>
+  <si>
+    <t>19.18</t>
+  </si>
+  <si>
+    <t>1.82</t>
+  </si>
+  <si>
+    <t>17.77</t>
+  </si>
+  <si>
+    <t>6.3</t>
+  </si>
+  <si>
+    <t>99.2</t>
+  </si>
+  <si>
+    <t>6.2</t>
+  </si>
+  <si>
+    <t>80.6</t>
+  </si>
+  <si>
+    <t>hibisco</t>
+  </si>
+  <si>
+    <t>0.96</t>
+  </si>
+  <si>
+    <t>11.31</t>
+  </si>
+  <si>
+    <t>3.29</t>
+  </si>
+  <si>
+    <t>6.8</t>
+  </si>
+  <si>
+    <t>8.41</t>
+  </si>
+  <si>
+    <t>13.3</t>
+  </si>
+  <si>
+    <t>3.75</t>
+  </si>
+  <si>
+    <t>14.89</t>
+  </si>
+  <si>
+    <t>31.8</t>
+  </si>
+  <si>
+    <t>27.4</t>
+  </si>
+  <si>
+    <t>4.8</t>
+  </si>
+  <si>
+    <t>0.94</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>11.75</t>
+  </si>
+  <si>
+    <t>53.2</t>
+  </si>
+  <si>
+    <t>5.25</t>
+  </si>
+  <si>
+    <t>32.78</t>
+  </si>
+  <si>
+    <t>0.33</t>
+  </si>
+  <si>
+    <t>1.36</t>
+  </si>
+  <si>
+    <t>38.06</t>
+  </si>
+  <si>
+    <t>20.6</t>
+  </si>
+  <si>
+    <t>0.82</t>
+  </si>
+  <si>
+    <t>14.98</t>
+  </si>
+  <si>
+    <t>36.4</t>
+  </si>
+  <si>
+    <t>3.15</t>
+  </si>
+  <si>
+    <t>2.65</t>
+  </si>
+  <si>
+    <t>37.8</t>
+  </si>
+  <si>
+    <t>9.6</t>
+  </si>
+  <si>
+    <t>48.8</t>
+  </si>
+  <si>
+    <t>0.67</t>
+  </si>
+  <si>
+    <t>7.68</t>
+  </si>
+  <si>
+    <t>58.8</t>
+  </si>
+  <si>
+    <t>pimenta-cambuci</t>
+  </si>
+  <si>
+    <t>31.60</t>
+  </si>
+  <si>
+    <t>185.8</t>
+  </si>
+  <si>
+    <t>39.1</t>
+  </si>
+  <si>
+    <t>28.4</t>
+  </si>
+  <si>
+    <t>4.14</t>
+  </si>
+  <si>
+    <t>13.21</t>
+  </si>
+  <si>
+    <t>4.23</t>
+  </si>
+  <si>
+    <t>41.85</t>
+  </si>
+  <si>
+    <t>7.08</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>3.74</t>
+  </si>
+  <si>
+    <t>9.5</t>
+  </si>
+  <si>
+    <t>0.86</t>
+  </si>
+  <si>
+    <t>4.64</t>
+  </si>
+  <si>
+    <t>80.4</t>
+  </si>
+  <si>
+    <t>0.68</t>
+  </si>
+  <si>
+    <t>14.8</t>
+  </si>
+  <si>
+    <t>2.58</t>
+  </si>
+  <si>
+    <t>3.65</t>
+  </si>
+  <si>
+    <t>0.69</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>6.33</t>
+  </si>
+  <si>
+    <t>0.88</t>
+  </si>
+  <si>
+    <t>3.89</t>
+  </si>
+  <si>
+    <t>13.7</t>
+  </si>
+  <si>
+    <t>18.6</t>
+  </si>
+  <si>
+    <t>21.2</t>
+  </si>
+  <si>
+    <t>tomate 
+cereja</t>
+  </si>
+  <si>
+    <t>alface
+crespa</t>
+  </si>
+  <si>
+    <t>alho
+poró</t>
+  </si>
+  <si>
+    <t>banana
+pão</t>
+  </si>
+  <si>
+    <t>banana
+nanica</t>
+  </si>
+  <si>
+    <t>banana
+prata</t>
+  </si>
+  <si>
+    <t>batata
+tupinambo</t>
+  </si>
+  <si>
+    <t>couve
+manteiga</t>
+  </si>
+  <si>
+    <t>ervilha
+torta</t>
+  </si>
+  <si>
+    <t>feijão
+guandu
+(verde)</t>
+  </si>
+  <si>
+    <t>feijão
+guandu
+(seco)</t>
+  </si>
+  <si>
+    <t>goiaba
+branca</t>
+  </si>
+  <si>
+    <t>goiaba
+vermelha</t>
+  </si>
+  <si>
+    <t>hortelã
+pimenta</t>
+  </si>
+  <si>
+    <t>limão
+cravo
+(suco)</t>
+  </si>
+  <si>
+    <t>mexerica
+ponkan</t>
+  </si>
+  <si>
+    <t>pimenta
+biquinho</t>
+  </si>
+  <si>
+    <t>proteínas (g)</t>
+  </si>
+  <si>
+    <t>fibras (g)</t>
+  </si>
+  <si>
+    <t>carboidratos (g)</t>
+  </si>
+  <si>
+    <t>caqui</t>
   </si>
 </sst>
 </file>
@@ -510,11 +893,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -831,8 +1217,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C165D6F-8FA7-44DB-A078-36B533BEFB91}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,7 +1371,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
@@ -1067,7 +1454,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>164</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
@@ -1314,82 +1701,106 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A844EE-D887-4A6B-B86C-B7C752CAF55A}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" t="s">
         <v>46</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" t="s">
         <v>47</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72601697-55EE-475A-BC70-2B6BB9EC57DD}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B3" t="s">
-        <v>142</v>
+      <c r="B4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1399,40 +1810,41 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF289E3-7000-4F49-BDDB-76D25F29B57D}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1443,16 +1855,16 @@
         <v>32</v>
       </c>
       <c r="C2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" t="s">
         <v>74</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>75</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>76</v>
-      </c>
-      <c r="F2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1463,13 +1875,13 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
         <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F3">
         <v>43</v>
@@ -1483,21 +1895,21 @@
         <v>131</v>
       </c>
       <c r="C4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
         <v>79</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>80</v>
       </c>
-      <c r="E4" t="s">
-        <v>81</v>
-      </c>
       <c r="F4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>245</v>
       </c>
       <c r="B5">
         <v>14</v>
@@ -1506,13 +1918,13 @@
         <v>53</v>
       </c>
       <c r="D5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" t="s">
         <v>82</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>83</v>
-      </c>
-      <c r="F5" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1520,36 +1932,36 @@
         <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" t="s">
         <v>85</v>
-      </c>
-      <c r="E6" t="s">
-        <v>86</v>
       </c>
       <c r="F6">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>27</v>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>246</v>
       </c>
       <c r="B7">
         <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" t="s">
         <v>88</v>
-      </c>
-      <c r="E7" t="s">
-        <v>89</v>
       </c>
       <c r="F7">
         <v>12</v>
@@ -1563,13 +1975,13 @@
         <v>43</v>
       </c>
       <c r="C8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" t="s">
         <v>90</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>91</v>
-      </c>
-      <c r="E8" t="s">
-        <v>92</v>
       </c>
       <c r="F8">
         <v>21</v>
@@ -1580,44 +1992,44 @@
         <v>32</v>
       </c>
       <c r="B9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" t="s">
         <v>94</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>95</v>
-      </c>
-      <c r="E9" t="s">
-        <v>96</v>
       </c>
       <c r="F9">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="B10">
         <v>105</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" t="s">
         <v>97</v>
       </c>
-      <c r="F10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>67</v>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>248</v>
       </c>
       <c r="B11">
         <v>92</v>
@@ -1629,21 +2041,21 @@
         <v>51</v>
       </c>
       <c r="E11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" t="s">
         <v>100</v>
       </c>
-      <c r="F11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>249</v>
       </c>
       <c r="B12">
         <v>98</v>
       </c>
       <c r="C12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -1652,12 +2064,12 @@
         <v>26</v>
       </c>
       <c r="F12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>56</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>250</v>
       </c>
       <c r="B13">
         <v>73</v>
@@ -1666,10 +2078,10 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" t="s">
         <v>103</v>
-      </c>
-      <c r="E13" t="s">
-        <v>104</v>
       </c>
       <c r="F13">
         <v>4</v>
@@ -1677,19 +2089,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>144</v>
       </c>
       <c r="B14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" t="s">
         <v>105</v>
-      </c>
-      <c r="D14" t="s">
-        <v>107</v>
-      </c>
-      <c r="E14" t="s">
-        <v>106</v>
       </c>
       <c r="F14">
         <v>102</v>
@@ -1703,16 +2115,16 @@
         <v>43</v>
       </c>
       <c r="C15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" t="s">
         <v>109</v>
       </c>
-      <c r="D15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>110</v>
-      </c>
-      <c r="F15" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1723,33 +2135,33 @@
         <v>34</v>
       </c>
       <c r="C16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" t="s">
         <v>112</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>113</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>114</v>
-      </c>
-      <c r="F16" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>145</v>
       </c>
       <c r="B17">
         <v>75</v>
       </c>
       <c r="C17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" t="s">
         <v>117</v>
-      </c>
-      <c r="D17" t="s">
-        <v>116</v>
-      </c>
-      <c r="E17" t="s">
-        <v>118</v>
       </c>
       <c r="F17">
         <v>2147</v>
@@ -1757,10 +2169,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1769,10 +2181,10 @@
         <v>52</v>
       </c>
       <c r="E18" t="s">
+        <v>119</v>
+      </c>
+      <c r="F18" t="s">
         <v>120</v>
-      </c>
-      <c r="F18" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1783,27 +2195,27 @@
         <v>32</v>
       </c>
       <c r="C19" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19" t="s">
         <v>122</v>
       </c>
-      <c r="D19" t="s">
-        <v>113</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>123</v>
-      </c>
-      <c r="F19" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>146</v>
       </c>
       <c r="B20">
         <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D20" t="s">
         <v>51</v>
@@ -1812,15 +2224,15 @@
         <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>147</v>
       </c>
       <c r="B21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C21">
         <f>1.05*100/70</f>
@@ -1830,7 +2242,7 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F21">
         <v>45</v>
@@ -1844,13 +2256,13 @@
         <v>23</v>
       </c>
       <c r="C22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D22" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" t="s">
         <v>129</v>
-      </c>
-      <c r="D22" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" t="s">
-        <v>130</v>
       </c>
       <c r="F22">
         <v>27</v>
@@ -1858,35 +2270,696 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>148</v>
       </c>
       <c r="B23" t="s">
+        <v>131</v>
+      </c>
+      <c r="C23" t="s">
+        <v>130</v>
+      </c>
+      <c r="D23" t="s">
         <v>132</v>
       </c>
-      <c r="C23" t="s">
-        <v>131</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>133</v>
-      </c>
-      <c r="E23" t="s">
-        <v>134</v>
       </c>
       <c r="F23">
         <v>2</v>
       </c>
     </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B24">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>151</v>
+      </c>
+      <c r="F24" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>154</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>4.92</v>
+      </c>
+      <c r="F25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26">
+        <v>310</v>
+      </c>
+      <c r="C26" t="s">
+        <v>156</v>
+      </c>
+      <c r="D26" t="s">
+        <v>157</v>
+      </c>
+      <c r="E26" t="s">
+        <v>158</v>
+      </c>
+      <c r="F26" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B27">
+        <v>88</v>
+      </c>
+      <c r="C27" t="s">
+        <v>161</v>
+      </c>
+      <c r="D27" t="s">
+        <v>160</v>
+      </c>
+      <c r="E27" t="s">
+        <v>162</v>
+      </c>
+      <c r="F27" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>164</v>
+      </c>
+      <c r="B28">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" t="s">
+        <v>165</v>
+      </c>
+      <c r="E28" t="s">
+        <v>166</v>
+      </c>
+      <c r="F28" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B29">
+        <v>569</v>
+      </c>
+      <c r="C29" t="s">
+        <v>172</v>
+      </c>
+      <c r="D29" t="s">
+        <v>171</v>
+      </c>
+      <c r="E29" t="s">
+        <v>170</v>
+      </c>
+      <c r="F29">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="B30">
+        <v>343</v>
+      </c>
+      <c r="C30" t="s">
+        <v>168</v>
+      </c>
+      <c r="D30">
+        <v>15</v>
+      </c>
+      <c r="E30" t="s">
+        <v>169</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>74</v>
+      </c>
+      <c r="C31" t="s">
+        <v>173</v>
+      </c>
+      <c r="D31" t="s">
+        <v>174</v>
+      </c>
+      <c r="E31" t="s">
+        <v>175</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32">
+        <v>80</v>
+      </c>
+      <c r="C32" t="s">
+        <v>176</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>177</v>
+      </c>
+      <c r="F32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B33">
+        <v>52</v>
+      </c>
+      <c r="C33" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" t="s">
+        <v>178</v>
+      </c>
+      <c r="E33" t="s">
+        <v>163</v>
+      </c>
+      <c r="F33" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B34">
+        <v>54</v>
+      </c>
+      <c r="C34" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E34">
+        <v>13</v>
+      </c>
+      <c r="F34" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>182</v>
+      </c>
+      <c r="B35">
+        <v>49</v>
+      </c>
+      <c r="C35" t="s">
+        <v>183</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>184</v>
+      </c>
+      <c r="F35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36">
+        <v>44</v>
+      </c>
+      <c r="C36" t="s">
+        <v>185</v>
+      </c>
+      <c r="D36" t="s">
+        <v>186</v>
+      </c>
+      <c r="E36" t="s">
+        <v>187</v>
+      </c>
+      <c r="F36" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B37">
+        <v>70</v>
+      </c>
+      <c r="C37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D37">
+        <v>8</v>
+      </c>
+      <c r="E37" t="s">
+        <v>190</v>
+      </c>
+      <c r="F37" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" t="s">
+        <v>192</v>
+      </c>
+      <c r="C38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" t="s">
+        <v>193</v>
+      </c>
+      <c r="E38" t="s">
+        <v>180</v>
+      </c>
+      <c r="F38" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39">
+        <v>47</v>
+      </c>
+      <c r="C39" t="s">
+        <v>194</v>
+      </c>
+      <c r="D39" t="s">
+        <v>195</v>
+      </c>
+      <c r="E39" t="s">
+        <v>196</v>
+      </c>
+      <c r="F39" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="B40" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" t="s">
+        <v>200</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>198</v>
+      </c>
+      <c r="F40" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41">
+        <v>160</v>
+      </c>
+      <c r="C41" t="s">
+        <v>201</v>
+      </c>
+      <c r="D41" t="s">
+        <v>87</v>
+      </c>
+      <c r="E41" t="s">
+        <v>202</v>
+      </c>
+      <c r="F41" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42">
+        <v>60</v>
+      </c>
+      <c r="C42" t="s">
+        <v>204</v>
+      </c>
+      <c r="D42" t="s">
+        <v>102</v>
+      </c>
+      <c r="E42" t="s">
+        <v>205</v>
+      </c>
+      <c r="F42" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43">
+        <v>23</v>
+      </c>
+      <c r="C43" t="s">
+        <v>207</v>
+      </c>
+      <c r="D43" t="s">
+        <v>102</v>
+      </c>
+      <c r="E43" t="s">
+        <v>208</v>
+      </c>
+      <c r="F43">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B44" t="s">
+        <v>209</v>
+      </c>
+      <c r="C44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E44" t="s">
+        <v>210</v>
+      </c>
+      <c r="F44" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45">
+        <v>32</v>
+      </c>
+      <c r="C45" t="s">
+        <v>212</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45" t="s">
+        <v>213</v>
+      </c>
+      <c r="F45" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" t="s">
+        <v>216</v>
+      </c>
+      <c r="C46" t="s">
+        <v>219</v>
+      </c>
+      <c r="D46" t="s">
+        <v>218</v>
+      </c>
+      <c r="E46">
+        <v>5</v>
+      </c>
+      <c r="F46" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" t="s">
+        <v>223</v>
+      </c>
+      <c r="C47" t="s">
+        <v>220</v>
+      </c>
+      <c r="D47" t="s">
+        <v>221</v>
+      </c>
+      <c r="E47" t="s">
+        <v>222</v>
+      </c>
+      <c r="F47" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B48">
+        <v>29</v>
+      </c>
+      <c r="C48" t="s">
+        <v>89</v>
+      </c>
+      <c r="D48" t="s">
+        <v>225</v>
+      </c>
+      <c r="E48" t="s">
+        <v>226</v>
+      </c>
+      <c r="F48">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>215</v>
+      </c>
+      <c r="B49">
+        <v>40</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49" t="s">
+        <v>87</v>
+      </c>
+      <c r="E49" t="s">
+        <v>227</v>
+      </c>
+      <c r="F49">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>38</v>
+      </c>
+      <c r="B50">
+        <v>20</v>
+      </c>
+      <c r="C50" t="s">
+        <v>228</v>
+      </c>
+      <c r="D50" t="s">
+        <v>52</v>
+      </c>
+      <c r="E50" t="s">
+        <v>229</v>
+      </c>
+      <c r="F50" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51">
+        <v>16</v>
+      </c>
+      <c r="C51" t="s">
+        <v>231</v>
+      </c>
+      <c r="D51" t="s">
+        <v>102</v>
+      </c>
+      <c r="E51" t="s">
+        <v>225</v>
+      </c>
+      <c r="F51" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52">
+        <v>25</v>
+      </c>
+      <c r="C52" t="s">
+        <v>233</v>
+      </c>
+      <c r="D52" t="s">
+        <v>102</v>
+      </c>
+      <c r="E52" t="s">
+        <v>234</v>
+      </c>
+      <c r="F52">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>39</v>
+      </c>
+      <c r="B53">
+        <v>16</v>
+      </c>
+      <c r="C53" t="s">
+        <v>235</v>
+      </c>
+      <c r="D53" t="s">
+        <v>102</v>
+      </c>
+      <c r="E53" t="s">
+        <v>82</v>
+      </c>
+      <c r="F53" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>20</v>
+      </c>
+      <c r="B54">
+        <v>36</v>
+      </c>
+      <c r="C54" t="s">
+        <v>82</v>
+      </c>
+      <c r="D54" t="s">
+        <v>237</v>
+      </c>
+      <c r="E54" t="s">
+        <v>238</v>
+      </c>
+      <c r="F54">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55">
+        <v>18</v>
+      </c>
+      <c r="C55" t="s">
+        <v>239</v>
+      </c>
+      <c r="D55" t="s">
+        <v>81</v>
+      </c>
+      <c r="E55" t="s">
+        <v>240</v>
+      </c>
+      <c r="F55" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="B56" t="s">
+        <v>242</v>
+      </c>
+      <c r="C56" t="s">
+        <v>53</v>
+      </c>
+      <c r="D56" t="s">
+        <v>81</v>
+      </c>
+      <c r="E56">
+        <v>4</v>
+      </c>
+      <c r="F56" t="s">
+        <v>243</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{139A8170-C326-48C9-9DB4-ACB9C17D90E1}">
-  <dimension ref="A1:A32"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1896,162 +2969,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>61</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualização da base e notebook
</commit_message>
<xml_diff>
--- a/data/csa_pindorama.xlsx
+++ b/data/csa_pindorama.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RNFAVAR.EMBAD.000\Documents\NEO DIPAS\Ciencia de Dados na Embraer\repos\web_app_CSA_pindorama\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF4EA68-059F-4B5F-BCFF-C46B5A300960}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492380D6-7BC3-4B46-B82D-026588C9F031}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28860" yWindow="-1860" windowWidth="28920" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="produtos" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="285">
   <si>
     <t>produto</t>
   </si>
@@ -864,9 +864,6 @@
     <t>plantio em geral</t>
   </si>
   <si>
-    <t xml:space="preserve"> Voluntários avisar no grupo (máx. 3 pessoas)</t>
-  </si>
-  <si>
     <t>data</t>
   </si>
   <si>
@@ -913,6 +910,9 @@
   </si>
   <si>
     <t>melaço de cana</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> voluntários avisar no grupo (máx. 3 pessoas)</t>
   </si>
 </sst>
 </file>
@@ -1278,9 +1278,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C65"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1319,7 +1319,9 @@
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1346,7 +1348,9 @@
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -1364,7 +1368,9 @@
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -1409,7 +1415,9 @@
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -1502,7 +1510,9 @@
       <c r="B23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="D23" s="14" t="s">
         <v>5</v>
       </c>
@@ -1550,7 +1560,9 @@
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
@@ -1702,7 +1714,9 @@
       <c r="B45" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="2"/>
+      <c r="C45" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
@@ -1736,7 +1750,7 @@
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
@@ -1868,7 +1882,9 @@
       <c r="B62" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C62" s="2"/>
+      <c r="C62" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="D62" s="5" t="s">
         <v>5</v>
       </c>
@@ -2846,7 +2862,7 @@
   <dimension ref="A1:C995"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2876,10 +2892,10 @@
         <v>44380</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2887,10 +2903,10 @@
         <v>44387</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2909,7 +2925,7 @@
         <v>44401</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>69</v>
@@ -2920,7 +2936,7 @@
         <v>44408</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>71</v>
@@ -3916,8 +3932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3950,7 +3966,29 @@
         <v>267</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>268</v>
+        <v>284</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="23">
+        <v>44395</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23">
+        <v>44409</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14656,7 +14694,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14668,15 +14706,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>21</v>
@@ -14684,7 +14722,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>49</v>
@@ -14692,7 +14730,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>64</v>
@@ -14700,7 +14738,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B5" s="25" t="s">
         <v>22</v>
@@ -14708,7 +14746,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B6" s="25" t="s">
         <v>26</v>
@@ -14716,7 +14754,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B7" s="25" t="s">
         <v>54</v>
@@ -14724,7 +14762,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B8" s="25" t="s">
         <v>60</v>
@@ -14732,7 +14770,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B9" s="25" t="s">
         <v>61</v>
@@ -14740,7 +14778,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B10" s="25" t="s">
         <v>62</v>
@@ -14748,7 +14786,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B11" s="25" t="s">
         <v>64</v>
@@ -14777,7 +14815,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>72</v>
@@ -14788,7 +14826,7 @@
         <v>44346</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -14796,7 +14834,7 @@
         <v>44350</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -14840,10 +14878,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>269</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -14907,7 +14945,7 @@
         <v>44345</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -14939,7 +14977,7 @@
         <v>44352</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -15091,7 +15129,7 @@
         <v>44359</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -15131,7 +15169,7 @@
         <v>44366</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
atualização da base e add img
</commit_message>
<xml_diff>
--- a/data/csa_pindorama.xlsx
+++ b/data/csa_pindorama.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RNFAVAR.EMBAD.000\Documents\NEO DIPAS\Ciencia de Dados na Embraer\repos\web_app_CSA_pindorama\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA00EF26-3DB2-45F0-9989-C9D3235FC2BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C46B9B5-66C7-4B15-A557-8E81696FC7EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8070" yWindow="2160" windowWidth="21600" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28860" yWindow="-1860" windowWidth="28920" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="produtos" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,9 @@
     <sheet name="hist_cestas" sheetId="6" r:id="rId4"/>
     <sheet name="qtde_cestas" sheetId="9" r:id="rId5"/>
     <sheet name="info_nutricional" sheetId="4" r:id="rId6"/>
-    <sheet name="info_nutricional_completar" sheetId="5" r:id="rId7"/>
-    <sheet name="hist_plantios" sheetId="8" r:id="rId8"/>
-    <sheet name="hist_mutiroes" sheetId="7" r:id="rId9"/>
+    <sheet name="hist_plantios" sheetId="8" r:id="rId7"/>
+    <sheet name="hist_mutiroes" sheetId="7" r:id="rId8"/>
+    <sheet name="info_nutricional_completar" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="297">
   <si>
     <t>produto</t>
   </si>
@@ -902,9 +902,6 @@
   </si>
   <si>
     <t>???</t>
-  </si>
-  <si>
-    <t>Josiane</t>
   </si>
   <si>
     <t xml:space="preserve">abobrinha </t>
@@ -962,11 +959,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/mmm"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1123,62 +1127,63 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="16" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1398,8 +1403,8 @@
   <dimension ref="A1:F1016"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C75"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1424,7 +1429,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>5</v>
@@ -1444,7 +1449,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>5</v>
@@ -1485,9 +1490,7 @@
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C7" s="2"/>
       <c r="D7" t="s">
         <v>5</v>
       </c>
@@ -1500,9 +1503,7 @@
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C8" s="2"/>
       <c r="D8" s="13" t="s">
         <v>5</v>
       </c>
@@ -1528,7 +1529,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>5</v>
@@ -1629,7 +1630,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>5</v>
@@ -1652,9 +1653,7 @@
       <c r="B24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C24" s="2"/>
       <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1671,7 +1670,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>5</v>
@@ -1720,9 +1719,7 @@
         <v>279</v>
       </c>
       <c r="B31" s="13"/>
-      <c r="C31" s="13" t="s">
-        <v>5</v>
-      </c>
+      <c r="C31" s="13"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
@@ -1731,9 +1728,7 @@
       <c r="B32" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="13" t="s">
-        <v>5</v>
-      </c>
+      <c r="C32" s="13"/>
       <c r="D32" s="13" t="s">
         <v>5</v>
       </c>
@@ -1775,9 +1770,7 @@
       <c r="B36" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
@@ -2004,7 +1997,7 @@
     </row>
     <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B61" s="13" t="s">
         <v>5</v>
@@ -2078,9 +2071,7 @@
       <c r="B68" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C68" s="2"/>
       <c r="D68" s="5" t="s">
         <v>5</v>
       </c>
@@ -2116,9 +2107,7 @@
       <c r="B71" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C71" s="2"/>
       <c r="D71" s="5"/>
     </row>
     <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3095,10 +3084,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C988"/>
+  <dimension ref="A1:C987"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3125,10 +3114,10 @@
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
-        <v>44429</v>
+        <v>44436</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>280</v>
@@ -3136,7 +3125,7 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
-        <v>44436</v>
+        <v>44443</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>280</v>
@@ -3145,6 +3134,29 @@
         <v>280</v>
       </c>
     </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>44450</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>44457</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4124,7 +4136,6 @@
     <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -4136,7 +4147,7 @@
   <dimension ref="A1:C996"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4160,6 +4171,12 @@
       <c r="C2" s="12" t="s">
         <v>69</v>
       </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
     </row>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5149,15 +5166,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC1E263-8857-40F8-80EA-E2B9223A60B4}">
-  <dimension ref="A1:B122"/>
+  <dimension ref="A1:B132"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A129" sqref="A129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.25" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.375" style="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.75" style="23" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9" style="23"/>
   </cols>
@@ -6136,6 +6153,86 @@
       </c>
       <c r="B122" s="13" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="24">
+        <v>44429</v>
+      </c>
+      <c r="B123" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="24">
+        <v>44429</v>
+      </c>
+      <c r="B124" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="24">
+        <v>44429</v>
+      </c>
+      <c r="B125" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="24">
+        <v>44429</v>
+      </c>
+      <c r="B126" s="13" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="24">
+        <v>44429</v>
+      </c>
+      <c r="B127" s="13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="24">
+        <v>44429</v>
+      </c>
+      <c r="B128" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="24">
+        <v>44429</v>
+      </c>
+      <c r="B129" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="24">
+        <v>44429</v>
+      </c>
+      <c r="B130" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="24">
+        <v>44429</v>
+      </c>
+      <c r="B131" s="39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="24">
+        <v>44429</v>
+      </c>
+      <c r="B132" s="39" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -6146,10 +6243,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E81ABCE-0B0E-4E06-8B44-AC66B8A5A776}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6162,7 +6259,7 @@
         <v>264</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -6259,6 +6356,14 @@
       </c>
       <c r="B13">
         <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="38">
+        <v>44429</v>
+      </c>
+      <c r="B14">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -6276,7 +6381,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="T31" sqref="T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14970,6 +15075,443 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C485FD73-227A-4AA7-8321-07690C89BAF0}">
+  <dimension ref="A1:B42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L59" sqref="L59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.75" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.625" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>277</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>277</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>277</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>277</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>277</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>277</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>277</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>277</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="B22" s="33" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="36" t="s">
+        <v>293</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="36" t="s">
+        <v>293</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="36" t="s">
+        <v>293</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="36" t="s">
+        <v>293</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="36" t="s">
+        <v>293</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="36" t="s">
+        <v>293</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="36" t="s">
+        <v>293</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="36" t="s">
+        <v>293</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="36" t="s">
+        <v>293</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="36" t="s">
+        <v>293</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="36" t="s">
+        <v>293</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="36" t="s">
+        <v>293</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="36" t="s">
+        <v>293</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="36" t="s">
+        <v>293</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="36" t="s">
+        <v>293</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="36" t="s">
+        <v>293</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DF9FF76-6587-4A82-A1EA-3E210EA83BFC}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="23"/>
+    <col min="2" max="2" width="54.375" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="24">
+        <v>44346</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="24">
+        <v>44350</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="24">
+        <v>44381</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="C4" s="13"/>
+    </row>
+    <row r="5" spans="1:3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
+        <v>44394</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="C5" s="13"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="24">
+        <v>44409</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="24"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A1000"/>
   <sheetViews>
@@ -15980,441 +16522,4 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C485FD73-227A-4AA7-8321-07690C89BAF0}">
-  <dimension ref="A1:B42"/>
-  <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.75" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.625" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="23"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>271</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
-        <v>272</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
-        <v>272</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
-        <v>272</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
-        <v>273</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
-        <v>273</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
-        <v>273</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
-        <v>273</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
-        <v>273</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
-        <v>273</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
-        <v>273</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
-        <v>277</v>
-      </c>
-      <c r="B12" s="29" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
-        <v>277</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
-        <v>277</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
-        <v>277</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
-        <v>277</v>
-      </c>
-      <c r="B16" s="29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
-        <v>277</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
-        <v>277</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
-        <v>277</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
-        <v>293</v>
-      </c>
-      <c r="B20" s="33" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
-        <v>293</v>
-      </c>
-      <c r="B21" s="33" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
-        <v>293</v>
-      </c>
-      <c r="B22" s="33" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
-        <v>293</v>
-      </c>
-      <c r="B23" s="33" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="35" t="s">
-        <v>293</v>
-      </c>
-      <c r="B24" s="33" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
-        <v>293</v>
-      </c>
-      <c r="B25" s="33" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="35" t="s">
-        <v>293</v>
-      </c>
-      <c r="B26" s="33" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
-        <v>294</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
-        <v>294</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="36" t="s">
-        <v>294</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="36" t="s">
-        <v>294</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="36" t="s">
-        <v>294</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
-        <v>294</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="36" t="s">
-        <v>294</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="36" t="s">
-        <v>294</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="36" t="s">
-        <v>294</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="36" t="s">
-        <v>294</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="36" t="s">
-        <v>294</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="36" t="s">
-        <v>294</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="36" t="s">
-        <v>294</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="36" t="s">
-        <v>294</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="36" t="s">
-        <v>294</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="36" t="s">
-        <v>294</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DF9FF76-6587-4A82-A1EA-3E210EA83BFC}">
-  <dimension ref="A1:C9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9" style="23"/>
-    <col min="2" max="2" width="54.375" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="23"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>264</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="24">
-        <v>44346</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="24">
-        <v>44350</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="24">
-        <v>44381</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="C4" s="13"/>
-    </row>
-    <row r="5" spans="1:3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24">
-        <v>44394</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="C5" s="13"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="24">
-        <v>44409</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
upd da base pelo dsk
</commit_message>
<xml_diff>
--- a/data/csa_pindorama.xlsx
+++ b/data/csa_pindorama.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RNFAVAR.EMBAD.000\Documents\NEO DIPAS\Ciencia de Dados na Embraer\repos\web_app_CSA_pindorama\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE3EF26-5C29-4005-A7E8-DD7A3C8A0FDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454DE85B-1136-4785-925E-720CF64F9A61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28860" yWindow="-3555" windowWidth="28920" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="305">
   <si>
     <t>produto</t>
   </si>
@@ -955,18 +955,12 @@
     <t>Ana Carolina</t>
   </si>
   <si>
-    <t>Ana Beatriz</t>
-  </si>
-  <si>
     <t>Renato/Marina</t>
   </si>
   <si>
     <t>Bernadete</t>
   </si>
   <si>
-    <t>Débora/Humberto</t>
-  </si>
-  <si>
     <t>06/09/21 a 12/09/21</t>
   </si>
   <si>
@@ -977,6 +971,9 @@
   </si>
   <si>
     <t>cogumelo shimeji</t>
+  </si>
+  <si>
+    <t>pepino verde comprido</t>
   </si>
 </sst>
 </file>
@@ -986,11 +983,25 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/mmm"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1168,62 +1179,64 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="16" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="16" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1446,8 +1459,8 @@
   <dimension ref="A1:F1017"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I56" sqref="I56"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1527,9 +1540,7 @@
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C7" s="2"/>
       <c r="F7" s="33"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1552,9 +1563,7 @@
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="F9" s="33"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1562,9 +1571,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C10" s="2"/>
       <c r="F10" s="33"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1605,9 +1612,7 @@
       <c r="B14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -1757,7 +1762,7 @@
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -1809,9 +1814,7 @@
       <c r="B36" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
@@ -2059,7 +2062,7 @@
     </row>
     <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B64" s="13" t="s">
         <v>5</v>
@@ -2106,9 +2109,7 @@
       <c r="B68" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C68" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C68" s="3"/>
       <c r="D68" s="21"/>
     </row>
     <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2128,9 +2129,7 @@
       <c r="B70" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C70" s="2"/>
       <c r="D70" s="21"/>
     </row>
     <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2150,9 +2149,7 @@
       <c r="B72" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C72" s="2"/>
       <c r="D72" s="5" t="s">
         <v>5</v>
       </c>
@@ -2183,7 +2180,7 @@
     </row>
     <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B76" s="13" t="s">
         <v>5</v>
@@ -3141,10 +3138,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C985"/>
+  <dimension ref="A1:C984"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3171,32 +3168,32 @@
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
-        <v>44450</v>
+        <v>44457</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
-        <v>44457</v>
+        <v>44464</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
-        <v>44464</v>
+        <v>44471</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>301</v>
+        <v>280</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>280</v>
@@ -3204,7 +3201,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
-        <v>44471</v>
+        <v>44478</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>280</v>
@@ -4191,7 +4188,6 @@
     <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -5222,10 +5218,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC1E263-8857-40F8-80EA-E2B9223A60B4}">
-  <dimension ref="A1:B152"/>
+  <dimension ref="A1:B162"/>
   <sheetViews>
     <sheetView topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="A152" sqref="A152"/>
+      <selection activeCell="B167" sqref="B167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6449,6 +6445,86 @@
       </c>
       <c r="B152" s="40" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="24">
+        <v>44450</v>
+      </c>
+      <c r="B153" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="24">
+        <v>44450</v>
+      </c>
+      <c r="B154" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="24">
+        <v>44450</v>
+      </c>
+      <c r="B155" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="24">
+        <v>44450</v>
+      </c>
+      <c r="B156" s="4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="24">
+        <v>44450</v>
+      </c>
+      <c r="B157" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="24">
+        <v>44450</v>
+      </c>
+      <c r="B158" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="24">
+        <v>44450</v>
+      </c>
+      <c r="B159" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="24">
+        <v>44450</v>
+      </c>
+      <c r="B160" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="24">
+        <v>44450</v>
+      </c>
+      <c r="B161" s="43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="24">
+        <v>44450</v>
+      </c>
+      <c r="B162" s="13" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -15311,7 +15387,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15687,7 +15763,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="41" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B44" s="41" t="s">
         <v>13</v>
@@ -15698,7 +15774,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="41" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B45" s="41" t="s">
         <v>21</v>
@@ -15709,7 +15785,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="41" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B46" s="41" t="s">
         <v>9</v>
@@ -15720,7 +15796,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="41" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B47" s="41" t="s">
         <v>63</v>
@@ -15731,10 +15807,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="41" t="s">
-        <v>302</v>
-      </c>
-      <c r="B48" s="41" t="s">
-        <v>303</v>
+        <v>300</v>
+      </c>
+      <c r="B48" s="42" t="s">
+        <v>304</v>
       </c>
       <c r="C48" s="23">
         <v>50</v>
@@ -15742,10 +15818,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="41" t="s">
+        <v>300</v>
+      </c>
+      <c r="B49" s="41" t="s">
         <v>302</v>
-      </c>
-      <c r="B49" s="41" t="s">
-        <v>304</v>
       </c>
       <c r="C49" s="23">
         <v>100</v>
@@ -15753,7 +15829,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="41" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B50" s="41" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
upd da base e do app
</commit_message>
<xml_diff>
--- a/data/csa_pindorama.xlsx
+++ b/data/csa_pindorama.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RNFAVAR.EMBAD.000\Documents\NEO DIPAS\Ciencia de Dados na Embraer\repos\web_app_CSA_pindorama\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC0031E-F262-4C9C-9FBA-EA4B11554400}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6498A4-DBF5-4264-971D-F61607DB6BF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28860" yWindow="-3375" windowWidth="28920" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15660" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="produtos" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="309">
   <si>
     <t>produto</t>
   </si>
@@ -995,11 +995,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/mmm"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1212,62 +1219,63 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="16" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="16" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1494,9 +1502,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1526,9 +1534,7 @@
       <c r="B2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>5</v>
-      </c>
+      <c r="C2" s="13"/>
       <c r="D2" s="13" t="s">
         <v>5</v>
       </c>
@@ -1560,9 +1566,7 @@
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C5" s="2"/>
       <c r="F5" s="33"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1655,9 +1659,7 @@
       <c r="B14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -1675,9 +1677,7 @@
       <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
@@ -1747,9 +1747,7 @@
       <c r="B24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C24" s="2"/>
       <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1819,9 +1817,7 @@
       <c r="B31" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="13" t="s">
-        <v>5</v>
-      </c>
+      <c r="C31" s="13"/>
       <c r="D31" s="21"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1874,9 +1870,7 @@
       <c r="B36" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
@@ -1915,9 +1909,7 @@
       <c r="B40" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C40" s="2"/>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
@@ -2133,9 +2125,7 @@
       <c r="B64" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C64" s="2"/>
     </row>
     <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
@@ -3225,7 +3215,7 @@
   <dimension ref="A1:C981"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5299,10 +5289,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC1E263-8857-40F8-80EA-E2B9223A60B4}">
-  <dimension ref="A1:B193"/>
+  <dimension ref="A1:B211"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="B167" sqref="B167"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="E190" sqref="E190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6856,6 +6846,140 @@
         <v>63</v>
       </c>
     </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="24">
+        <v>44478</v>
+      </c>
+      <c r="B194" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="24">
+        <v>44478</v>
+      </c>
+      <c r="B195" s="13" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" s="24">
+        <v>44478</v>
+      </c>
+      <c r="B196" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" s="24">
+        <v>44478</v>
+      </c>
+      <c r="B197" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" s="24">
+        <v>44478</v>
+      </c>
+      <c r="B198" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" s="24">
+        <v>44478</v>
+      </c>
+      <c r="B199" s="13" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" s="24">
+        <v>44478</v>
+      </c>
+      <c r="B200" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" s="24">
+        <v>44478</v>
+      </c>
+      <c r="B201" s="13" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" s="24">
+        <v>44478</v>
+      </c>
+      <c r="B202" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" s="24">
+        <v>44478</v>
+      </c>
+      <c r="B203" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" s="24">
+        <v>44478</v>
+      </c>
+      <c r="B204" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" s="24">
+        <v>44478</v>
+      </c>
+      <c r="B205" s="13" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" s="24">
+        <v>44478</v>
+      </c>
+      <c r="B206" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" s="24">
+        <v>44478</v>
+      </c>
+      <c r="B207" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" s="24">
+        <v>44478</v>
+      </c>
+      <c r="B208" s="47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" s="24">
+        <v>44478</v>
+      </c>
+      <c r="B209" s="47" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" s="24"/>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" s="24"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6864,10 +6988,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E81ABCE-0B0E-4E06-8B44-AC66B8A5A776}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F38" sqref="F37:F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7033,6 +7157,14 @@
       </c>
       <c r="B20">
         <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="38">
+        <v>44478</v>
+      </c>
+      <c r="B21">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -15748,7 +15880,7 @@
   <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+      <selection activeCell="B55" sqref="B55:B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>